<commit_message>
burden_data, health_data, and clean_xlsx
</commit_message>
<xml_diff>
--- a/powerbi/waqi_data.xlsx
+++ b/powerbi/waqi_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1352,16 +1352,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>45759.16666666666</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1374,19 +1374,19 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2.7</v>
+        <v>13.3</v>
       </c>
       <c r="H20" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I20" t="n">
-        <v>1014.9</v>
+        <v>1035.1</v>
       </c>
       <c r="J20" t="n">
-        <v>11</v>
+        <v>0.6</v>
       </c>
       <c r="K20" t="n">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1394,21 +1394,21 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45759.20833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1421,45 +1421,45 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2.9</v>
+        <v>13.3</v>
       </c>
       <c r="H21" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I21" t="n">
-        <v>1014.7</v>
+        <v>1035.1</v>
       </c>
       <c r="J21" t="n">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="K21" t="n">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D22" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1468,45 +1468,45 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>10</v>
+        <v>13.3</v>
       </c>
       <c r="H22" t="n">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="I22" t="n">
-        <v>1009</v>
+        <v>1035.1</v>
       </c>
       <c r="J22" t="n">
-        <v>14.9</v>
+        <v>0.6</v>
       </c>
       <c r="K22" t="n">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>68</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D23" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1515,45 +1515,45 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>10</v>
+        <v>13.3</v>
       </c>
       <c r="H23" t="n">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="I23" t="n">
-        <v>1009</v>
+        <v>1035.1</v>
       </c>
       <c r="J23" t="n">
-        <v>14.9</v>
+        <v>0.6</v>
       </c>
       <c r="K23" t="n">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>74</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D24" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1562,45 +1562,45 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>10</v>
+        <v>13.3</v>
       </c>
       <c r="H24" t="n">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="I24" t="n">
-        <v>1009</v>
+        <v>1035.1</v>
       </c>
       <c r="J24" t="n">
-        <v>14.9</v>
+        <v>0.6</v>
       </c>
       <c r="K24" t="n">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>34.2</v>
+        <v>17.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D25" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1609,45 +1609,45 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>10</v>
+        <v>13.3</v>
       </c>
       <c r="H25" t="n">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="I25" t="n">
-        <v>1009</v>
+        <v>1035.1</v>
       </c>
       <c r="J25" t="n">
-        <v>14.9</v>
+        <v>0.6</v>
       </c>
       <c r="K25" t="n">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>1.9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.16666666666</v>
       </c>
       <c r="D26" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1656,45 +1656,45 @@
         </is>
       </c>
       <c r="G26" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="H26" t="n">
+        <v>97</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1014.9</v>
+      </c>
+      <c r="J26" t="n">
+        <v>11</v>
+      </c>
+      <c r="K26" t="n">
+        <v>57</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
         <v>10</v>
-      </c>
-      <c r="H26" t="n">
-        <v>19</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1009</v>
-      </c>
-      <c r="J26" t="n">
-        <v>14.9</v>
-      </c>
-      <c r="K26" t="n">
-        <v>12</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>no2</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>1.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.20833333334</v>
       </c>
       <c r="D27" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1703,45 +1703,45 @@
         </is>
       </c>
       <c r="G27" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="H27" t="n">
+        <v>97</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1014.7</v>
+      </c>
+      <c r="J27" t="n">
+        <v>6</v>
+      </c>
+      <c r="K27" t="n">
+        <v>82</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
         <v>10</v>
-      </c>
-      <c r="H27" t="n">
-        <v>19</v>
-      </c>
-      <c r="I27" t="n">
-        <v>1009</v>
-      </c>
-      <c r="J27" t="n">
-        <v>14.9</v>
-      </c>
-      <c r="K27" t="n">
-        <v>13</v>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>so2</t>
-        </is>
-      </c>
-      <c r="M27" t="n">
-        <v>3.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.29166666666</v>
       </c>
       <c r="D28" t="n">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1750,19 +1750,19 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>10</v>
+        <v>3.3</v>
       </c>
       <c r="H28" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="I28" t="n">
-        <v>1009</v>
+        <v>1014.6</v>
       </c>
       <c r="J28" t="n">
-        <v>14.9</v>
+        <v>9</v>
       </c>
       <c r="K28" t="n">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -1770,21 +1770,21 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B29" t="n">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D29" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1809,29 +1809,29 @@
         <v>14.9</v>
       </c>
       <c r="K29" t="n">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B30" t="n">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D30" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1856,29 +1856,29 @@
         <v>14.9</v>
       </c>
       <c r="K30" t="n">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>32.9</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B31" t="n">
         <v>3</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D31" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1903,29 +1903,29 @@
         <v>14.9</v>
       </c>
       <c r="K31" t="n">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>1.9</v>
+        <v>34.2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B32" t="n">
         <v>3</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D32" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1950,11 +1950,11 @@
         <v>14.9</v>
       </c>
       <c r="K32" t="n">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M32" t="n">
@@ -1963,16 +1963,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B33" t="n">
         <v>3</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>45759.75</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D33" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1997,29 +1997,29 @@
         <v>14.9</v>
       </c>
       <c r="K33" t="n">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>3.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B34" t="n">
         <v>3</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D34" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2032,41 +2032,41 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H34" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="J34" t="n">
-        <v>11.3</v>
+        <v>14.9</v>
       </c>
       <c r="K34" t="n">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>74</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B35" t="n">
         <v>3</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D35" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2079,88 +2079,88 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H35" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="J35" t="n">
-        <v>11.3</v>
+        <v>14.9</v>
       </c>
       <c r="K35" t="n">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B36" t="n">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D36" t="n">
+        <v>75</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>10</v>
+      </c>
+      <c r="H36" t="n">
+        <v>19</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1009</v>
+      </c>
+      <c r="J36" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="K36" t="n">
         <v>84</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>pm10</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>waqi</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
-        <v>9</v>
-      </c>
-      <c r="H36" t="n">
-        <v>20</v>
-      </c>
-      <c r="I36" t="n">
-        <v>1010</v>
-      </c>
-      <c r="J36" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="K36" t="n">
-        <v>115</v>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>o3</t>
-        </is>
-      </c>
       <c r="M36" t="n">
-        <v>33.3</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B37" t="n">
         <v>3</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D37" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2173,41 +2173,41 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="J37" t="n">
-        <v>11.3</v>
+        <v>14.9</v>
       </c>
       <c r="K37" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>1.9</v>
+        <v>32.9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B38" t="n">
         <v>3</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D38" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2220,41 +2220,41 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H38" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="J38" t="n">
-        <v>11.3</v>
+        <v>14.9</v>
       </c>
       <c r="K38" t="n">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B39" t="n">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>45759.79166666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D39" t="n">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2267,45 +2267,45 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H39" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39" t="n">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="J39" t="n">
-        <v>11.3</v>
+        <v>14.9</v>
       </c>
       <c r="K39" t="n">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.75</v>
       </c>
       <c r="D40" t="n">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2314,45 +2314,45 @@
         </is>
       </c>
       <c r="G40" t="n">
-        <v>32.8</v>
+        <v>10</v>
       </c>
       <c r="H40" t="n">
-        <v>37.05</v>
+        <v>19</v>
       </c>
       <c r="I40" t="n">
-        <v>981.3</v>
+        <v>1009</v>
       </c>
       <c r="J40" t="n">
-        <v>1.15</v>
+        <v>14.9</v>
       </c>
       <c r="K40" t="n">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>144</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D41" t="n">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2361,45 +2361,45 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>32.8</v>
+        <v>9</v>
       </c>
       <c r="H41" t="n">
-        <v>37.05</v>
+        <v>20</v>
       </c>
       <c r="I41" t="n">
-        <v>981.3</v>
+        <v>1010</v>
       </c>
       <c r="J41" t="n">
-        <v>1.15</v>
+        <v>11.3</v>
       </c>
       <c r="K41" t="n">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D42" t="n">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2408,45 +2408,45 @@
         </is>
       </c>
       <c r="G42" t="n">
-        <v>32.8</v>
+        <v>9</v>
       </c>
       <c r="H42" t="n">
-        <v>37.05</v>
+        <v>20</v>
       </c>
       <c r="I42" t="n">
-        <v>981.3</v>
+        <v>1010</v>
       </c>
       <c r="J42" t="n">
-        <v>1.15</v>
+        <v>11.3</v>
       </c>
       <c r="K42" t="n">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>94.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D43" t="n">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2455,45 +2455,45 @@
         </is>
       </c>
       <c r="G43" t="n">
-        <v>32.8</v>
+        <v>9</v>
       </c>
       <c r="H43" t="n">
-        <v>37.05</v>
+        <v>20</v>
       </c>
       <c r="I43" t="n">
-        <v>981.3</v>
+        <v>1010</v>
       </c>
       <c r="J43" t="n">
-        <v>1.15</v>
+        <v>11.3</v>
       </c>
       <c r="K43" t="n">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>5.2</v>
+        <v>33.3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D44" t="n">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2502,45 +2502,45 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>32.8</v>
+        <v>9</v>
       </c>
       <c r="H44" t="n">
-        <v>37.05</v>
+        <v>20</v>
       </c>
       <c r="I44" t="n">
-        <v>981.3</v>
+        <v>1010</v>
       </c>
       <c r="J44" t="n">
-        <v>1.15</v>
+        <v>11.3</v>
       </c>
       <c r="K44" t="n">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>8.9</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="2" t="n">
-        <v>45759.625</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D45" t="n">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2549,45 +2549,45 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>32.8</v>
+        <v>9</v>
       </c>
       <c r="H45" t="n">
-        <v>37.05</v>
+        <v>20</v>
       </c>
       <c r="I45" t="n">
-        <v>981.3</v>
+        <v>1010</v>
       </c>
       <c r="J45" t="n">
-        <v>1.15</v>
+        <v>11.3</v>
       </c>
       <c r="K45" t="n">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>8.6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.79166666666</v>
       </c>
       <c r="D46" t="n">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2596,45 +2596,45 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H46" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I46" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J46" t="n">
-        <v>1.05</v>
+        <v>11.3</v>
       </c>
       <c r="K46" t="n">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>124</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D47" t="n">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2643,45 +2643,45 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H47" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I47" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J47" t="n">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K47" t="n">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D48" t="n">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2690,45 +2690,45 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H48" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I48" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J48" t="n">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K48" t="n">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>78.2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D49" t="n">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2737,45 +2737,45 @@
         </is>
       </c>
       <c r="G49" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H49" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I49" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J49" t="n">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K49" t="n">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>4.6</v>
+        <v>32.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D50" t="n">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2784,45 +2784,45 @@
         </is>
       </c>
       <c r="G50" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H50" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I50" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J50" t="n">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K50" t="n">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>7.1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2" t="n">
-        <v>45759.66666666666</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D51" t="n">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2831,45 +2831,45 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>32.825</v>
+        <v>9</v>
       </c>
       <c r="H51" t="n">
-        <v>36.8</v>
+        <v>20</v>
       </c>
       <c r="I51" t="n">
-        <v>981.125</v>
+        <v>1010</v>
       </c>
       <c r="J51" t="n">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K51" t="n">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>6.5</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.83333333334</v>
       </c>
       <c r="D52" t="n">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2878,41 +2878,41 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>32.275</v>
+        <v>9</v>
       </c>
       <c r="H52" t="n">
-        <v>37.325</v>
+        <v>20</v>
       </c>
       <c r="I52" t="n">
-        <v>980.9</v>
+        <v>1010</v>
       </c>
       <c r="J52" t="n">
-        <v>0.6</v>
+        <v>11.8</v>
       </c>
       <c r="K52" t="n">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>95</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B53" t="n">
         <v>4</v>
       </c>
       <c r="C53" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D53" t="n">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2925,41 +2925,41 @@
         </is>
       </c>
       <c r="G53" t="n">
-        <v>32.275</v>
+        <v>32.8</v>
       </c>
       <c r="H53" t="n">
-        <v>37.325</v>
+        <v>37.05</v>
       </c>
       <c r="I53" t="n">
-        <v>980.9</v>
+        <v>981.3</v>
       </c>
       <c r="J53" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="K53" t="n">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>67</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B54" t="n">
         <v>4</v>
       </c>
       <c r="C54" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D54" t="n">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2972,41 +2972,41 @@
         </is>
       </c>
       <c r="G54" t="n">
-        <v>32.275</v>
+        <v>32.8</v>
       </c>
       <c r="H54" t="n">
-        <v>37.325</v>
+        <v>37.05</v>
       </c>
       <c r="I54" t="n">
-        <v>980.9</v>
+        <v>981.3</v>
       </c>
       <c r="J54" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="K54" t="n">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>75.5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B55" t="n">
         <v>4</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D55" t="n">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -3019,41 +3019,41 @@
         </is>
       </c>
       <c r="G55" t="n">
-        <v>32.275</v>
+        <v>32.8</v>
       </c>
       <c r="H55" t="n">
-        <v>37.325</v>
+        <v>37.05</v>
       </c>
       <c r="I55" t="n">
-        <v>980.9</v>
+        <v>981.3</v>
       </c>
       <c r="J55" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="K55" t="n">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>4.3</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B56" t="n">
         <v>4</v>
       </c>
       <c r="C56" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D56" t="n">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -3066,41 +3066,41 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>32.275</v>
+        <v>32.8</v>
       </c>
       <c r="H56" t="n">
-        <v>37.325</v>
+        <v>37.05</v>
       </c>
       <c r="I56" t="n">
-        <v>980.9</v>
+        <v>981.3</v>
       </c>
       <c r="J56" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="K56" t="n">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>7.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B57" t="n">
         <v>4</v>
       </c>
       <c r="C57" s="2" t="n">
-        <v>45759.70833333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D57" t="n">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -3113,41 +3113,41 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>32.275</v>
+        <v>32.8</v>
       </c>
       <c r="H57" t="n">
-        <v>37.325</v>
+        <v>37.05</v>
       </c>
       <c r="I57" t="n">
-        <v>980.9</v>
+        <v>981.3</v>
       </c>
       <c r="J57" t="n">
-        <v>0.6</v>
+        <v>1.15</v>
       </c>
       <c r="K57" t="n">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>6</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.625</v>
       </c>
       <c r="D58" t="n">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -3160,41 +3160,41 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>16.1</v>
+        <v>32.8</v>
       </c>
       <c r="H58" t="n">
-        <v>48.6</v>
+        <v>37.05</v>
       </c>
       <c r="I58" t="n">
-        <v>1009.4</v>
+        <v>981.3</v>
       </c>
       <c r="J58" t="n">
-        <v>0.2</v>
+        <v>1.15</v>
       </c>
       <c r="K58" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>70</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D59" t="n">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -3207,41 +3207,41 @@
         </is>
       </c>
       <c r="G59" t="n">
-        <v>16.1</v>
+        <v>32.825</v>
       </c>
       <c r="H59" t="n">
-        <v>48.6</v>
+        <v>36.8</v>
       </c>
       <c r="I59" t="n">
-        <v>1009.4</v>
+        <v>981.125</v>
       </c>
       <c r="J59" t="n">
-        <v>0.2</v>
+        <v>1.05</v>
       </c>
       <c r="K59" t="n">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>29</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D60" t="n">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -3254,41 +3254,41 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>16.1</v>
+        <v>32.825</v>
       </c>
       <c r="H60" t="n">
-        <v>48.6</v>
+        <v>36.8</v>
       </c>
       <c r="I60" t="n">
-        <v>1009.4</v>
+        <v>981.125</v>
       </c>
       <c r="J60" t="n">
-        <v>0.2</v>
+        <v>1.05</v>
       </c>
       <c r="K60" t="n">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>27.8</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D61" t="n">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -3301,41 +3301,41 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>16.1</v>
+        <v>32.825</v>
       </c>
       <c r="H61" t="n">
-        <v>48.6</v>
+        <v>36.8</v>
       </c>
       <c r="I61" t="n">
-        <v>1009.4</v>
+        <v>981.125</v>
       </c>
       <c r="J61" t="n">
-        <v>0.2</v>
+        <v>1.05</v>
       </c>
       <c r="K61" t="n">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>0.1</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D62" t="n">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -3348,41 +3348,41 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>16.1</v>
+        <v>32.825</v>
       </c>
       <c r="H62" t="n">
-        <v>48.6</v>
+        <v>36.8</v>
       </c>
       <c r="I62" t="n">
-        <v>1009.4</v>
+        <v>981.125</v>
       </c>
       <c r="J62" t="n">
-        <v>0.2</v>
+        <v>1.05</v>
       </c>
       <c r="K62" t="n">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>33.6</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" s="2" t="n">
-        <v>45759.33333333334</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D63" t="n">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -3395,41 +3395,41 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>16.1</v>
+        <v>32.825</v>
       </c>
       <c r="H63" t="n">
-        <v>48.6</v>
+        <v>36.8</v>
       </c>
       <c r="I63" t="n">
-        <v>1009.4</v>
+        <v>981.125</v>
       </c>
       <c r="J63" t="n">
-        <v>0.2</v>
+        <v>1.05</v>
       </c>
       <c r="K63" t="n">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>0.6</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.66666666666</v>
       </c>
       <c r="D64" t="n">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -3442,41 +3442,41 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>18.7</v>
+        <v>32.825</v>
       </c>
       <c r="H64" t="n">
-        <v>45</v>
+        <v>36.8</v>
       </c>
       <c r="I64" t="n">
-        <v>1008.7</v>
+        <v>981.125</v>
       </c>
       <c r="J64" t="n">
-        <v>1.2</v>
+        <v>1.05</v>
       </c>
       <c r="K64" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>63</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D65" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -3489,41 +3489,41 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>18.7</v>
+        <v>32.275</v>
       </c>
       <c r="H65" t="n">
-        <v>45</v>
+        <v>37.325</v>
       </c>
       <c r="I65" t="n">
-        <v>1008.7</v>
+        <v>980.9</v>
       </c>
       <c r="J65" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="K65" t="n">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>24</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D66" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -3536,41 +3536,41 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>18.7</v>
+        <v>32.275</v>
       </c>
       <c r="H66" t="n">
-        <v>45</v>
+        <v>37.325</v>
       </c>
       <c r="I66" t="n">
-        <v>1008.7</v>
+        <v>980.9</v>
       </c>
       <c r="J66" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="K66" t="n">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>o3</t>
+          <t>pm10</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>30.7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C67" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D67" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -3583,41 +3583,41 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>18.7</v>
+        <v>32.275</v>
       </c>
       <c r="H67" t="n">
-        <v>45</v>
+        <v>37.325</v>
       </c>
       <c r="I67" t="n">
-        <v>1008.7</v>
+        <v>980.9</v>
       </c>
       <c r="J67" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="K67" t="n">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>0.1</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B68" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D68" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3630,41 +3630,41 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>18.7</v>
+        <v>32.275</v>
       </c>
       <c r="H68" t="n">
-        <v>45</v>
+        <v>37.325</v>
       </c>
       <c r="I68" t="n">
-        <v>1008.7</v>
+        <v>980.9</v>
       </c>
       <c r="J68" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="K68" t="n">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>29</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>45759.375</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D69" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -3677,45 +3677,45 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>18.7</v>
+        <v>32.275</v>
       </c>
       <c r="H69" t="n">
-        <v>45</v>
+        <v>37.325</v>
       </c>
       <c r="I69" t="n">
-        <v>1008.7</v>
+        <v>980.9</v>
       </c>
       <c r="J69" t="n">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="K69" t="n">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>so2</t>
+          <t>no2</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>0.6</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>45759.41666666666</v>
+        <v>45759.70833333334</v>
       </c>
       <c r="D70" t="n">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3724,45 +3724,45 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>18.3</v>
+        <v>32.275</v>
       </c>
       <c r="H70" t="n">
-        <v>45.5</v>
+        <v>37.325</v>
       </c>
       <c r="I70" t="n">
-        <v>1008.8</v>
+        <v>980.9</v>
       </c>
       <c r="J70" t="n">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
       <c r="K70" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>pm25</t>
+          <t>so2</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>45759.41666666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D71" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3771,92 +3771,92 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>18.3</v>
+        <v>31.45</v>
       </c>
       <c r="H71" t="n">
-        <v>45.5</v>
+        <v>39.25</v>
       </c>
       <c r="I71" t="n">
-        <v>1008.8</v>
+        <v>981.2</v>
       </c>
       <c r="J71" t="n">
-        <v>1.5</v>
+        <v>0.65</v>
       </c>
       <c r="K71" t="n">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>45759.41666666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D72" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>31.45</v>
+      </c>
+      <c r="H72" t="n">
+        <v>39.25</v>
+      </c>
+      <c r="I72" t="n">
+        <v>981.2</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K72" t="n">
+        <v>139</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
           <t>pm10</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>waqi</t>
-        </is>
-      </c>
-      <c r="G72" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="H72" t="n">
-        <v>45.5</v>
-      </c>
-      <c r="I72" t="n">
-        <v>1008.8</v>
-      </c>
-      <c r="J72" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K72" t="n">
-        <v>97</v>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>o3</t>
-        </is>
-      </c>
       <c r="M72" t="n">
-        <v>17.6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>45759.41666666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D73" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3865,45 +3865,45 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>18.3</v>
+        <v>31.45</v>
       </c>
       <c r="H73" t="n">
-        <v>45.5</v>
+        <v>39.25</v>
       </c>
       <c r="I73" t="n">
-        <v>1008.8</v>
+        <v>981.2</v>
       </c>
       <c r="J73" t="n">
-        <v>1.5</v>
+        <v>0.65</v>
       </c>
       <c r="K73" t="n">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>co</t>
+          <t>o3</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>0.1</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>45759.41666666666</v>
+        <v>45759.75</v>
       </c>
       <c r="D74" t="n">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>pm10</t>
+          <t>pm25</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3912,73 +3912,1248 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>18.3</v>
+        <v>31.45</v>
       </c>
       <c r="H74" t="n">
-        <v>45.5</v>
+        <v>39.25</v>
       </c>
       <c r="I74" t="n">
-        <v>1008.8</v>
+        <v>981.2</v>
       </c>
       <c r="J74" t="n">
-        <v>1.5</v>
+        <v>0.65</v>
       </c>
       <c r="K74" t="n">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>no2</t>
+          <t>co</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>29</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
+        <v>28</v>
+      </c>
+      <c r="B75" t="n">
+        <v>4</v>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>45759.75</v>
+      </c>
+      <c r="D75" t="n">
+        <v>99</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>31.45</v>
+      </c>
+      <c r="H75" t="n">
+        <v>39.25</v>
+      </c>
+      <c r="I75" t="n">
+        <v>981.2</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K75" t="n">
+        <v>142</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>no2</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>28</v>
+      </c>
+      <c r="B76" t="n">
+        <v>4</v>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>45759.75</v>
+      </c>
+      <c r="D76" t="n">
+        <v>99</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>31.45</v>
+      </c>
+      <c r="H76" t="n">
+        <v>39.25</v>
+      </c>
+      <c r="I76" t="n">
+        <v>981.2</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K76" t="n">
+        <v>143</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>so2</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>5</v>
+      </c>
+      <c r="B77" t="n">
+        <v>5</v>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D77" t="n">
+        <v>70</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H77" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I77" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K77" t="n">
         <v>20</v>
       </c>
-      <c r="B75" t="n">
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
         <v>5</v>
       </c>
-      <c r="C75" s="2" t="n">
+      <c r="B78" t="n">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D78" t="n">
+        <v>70</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H78" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I78" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K78" t="n">
+        <v>21</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>5</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5</v>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D79" t="n">
+        <v>70</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I79" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K79" t="n">
+        <v>22</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>5</v>
+      </c>
+      <c r="B80" t="n">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D80" t="n">
+        <v>70</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H80" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I80" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K80" t="n">
+        <v>23</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>5</v>
+      </c>
+      <c r="B81" t="n">
+        <v>5</v>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D81" t="n">
+        <v>70</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H81" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I81" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K81" t="n">
+        <v>24</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>no2</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>5</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>45759.33333333334</v>
+      </c>
+      <c r="D82" t="n">
+        <v>70</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="H82" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1009.4</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K82" t="n">
+        <v>25</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>so2</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>21</v>
+      </c>
+      <c r="B83" t="n">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D83" t="n">
+        <v>63</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H83" t="n">
+        <v>45</v>
+      </c>
+      <c r="I83" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J83" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K83" t="n">
+        <v>101</v>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>21</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D84" t="n">
+        <v>63</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H84" t="n">
+        <v>45</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J84" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K84" t="n">
+        <v>102</v>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>21</v>
+      </c>
+      <c r="B85" t="n">
+        <v>5</v>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D85" t="n">
+        <v>63</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H85" t="n">
+        <v>45</v>
+      </c>
+      <c r="I85" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J85" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K85" t="n">
+        <v>103</v>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>21</v>
+      </c>
+      <c r="B86" t="n">
+        <v>5</v>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D86" t="n">
+        <v>63</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H86" t="n">
+        <v>45</v>
+      </c>
+      <c r="I86" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J86" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K86" t="n">
+        <v>104</v>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>21</v>
+      </c>
+      <c r="B87" t="n">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D87" t="n">
+        <v>63</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H87" t="n">
+        <v>45</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K87" t="n">
+        <v>105</v>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>no2</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>21</v>
+      </c>
+      <c r="B88" t="n">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>45759.375</v>
+      </c>
+      <c r="D88" t="n">
+        <v>63</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H88" t="n">
+        <v>45</v>
+      </c>
+      <c r="I88" t="n">
+        <v>1008.7</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K88" t="n">
+        <v>106</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>so2</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>20</v>
+      </c>
+      <c r="B89" t="n">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="n">
         <v>45759.41666666666</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D89" t="n">
         <v>24</v>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t>pm10</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>waqi</t>
-        </is>
-      </c>
-      <c r="G75" t="n">
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
         <v>18.3</v>
       </c>
-      <c r="H75" t="n">
+      <c r="H89" t="n">
         <v>45.5</v>
       </c>
-      <c r="I75" t="n">
+      <c r="I89" t="n">
         <v>1008.8</v>
       </c>
-      <c r="J75" t="n">
+      <c r="J89" t="n">
         <v>1.5</v>
       </c>
-      <c r="K75" t="n">
+      <c r="K89" t="n">
+        <v>95</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>20</v>
+      </c>
+      <c r="B90" t="n">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>45759.41666666666</v>
+      </c>
+      <c r="D90" t="n">
+        <v>24</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H90" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I90" t="n">
+        <v>1008.8</v>
+      </c>
+      <c r="J90" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K90" t="n">
+        <v>96</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>20</v>
+      </c>
+      <c r="B91" t="n">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>45759.41666666666</v>
+      </c>
+      <c r="D91" t="n">
+        <v>24</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H91" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I91" t="n">
+        <v>1008.8</v>
+      </c>
+      <c r="J91" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K91" t="n">
+        <v>97</v>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>20</v>
+      </c>
+      <c r="B92" t="n">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>45759.41666666666</v>
+      </c>
+      <c r="D92" t="n">
+        <v>24</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H92" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I92" t="n">
+        <v>1008.8</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K92" t="n">
+        <v>98</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>20</v>
+      </c>
+      <c r="B93" t="n">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>45759.41666666666</v>
+      </c>
+      <c r="D93" t="n">
+        <v>24</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H93" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I93" t="n">
+        <v>1008.8</v>
+      </c>
+      <c r="J93" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K93" t="n">
+        <v>99</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>no2</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>20</v>
+      </c>
+      <c r="B94" t="n">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>45759.41666666666</v>
+      </c>
+      <c r="D94" t="n">
+        <v>24</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="H94" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="I94" t="n">
+        <v>1008.8</v>
+      </c>
+      <c r="J94" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K94" t="n">
         <v>100</v>
       </c>
-      <c r="L75" t="inlineStr">
+      <c r="L94" t="inlineStr">
         <is>
           <t>so2</t>
         </is>
       </c>
-      <c r="M75" t="n">
+      <c r="M94" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>29</v>
+      </c>
+      <c r="B95" t="n">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D95" t="n">
+        <v>33</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H95" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K95" t="n">
+        <v>144</v>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>29</v>
+      </c>
+      <c r="B96" t="n">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D96" t="n">
+        <v>33</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H96" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I96" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K96" t="n">
+        <v>145</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>pm10</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>29</v>
+      </c>
+      <c r="B97" t="n">
+        <v>5</v>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D97" t="n">
+        <v>33</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H97" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I97" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K97" t="n">
+        <v>146</v>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="M97" t="n">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>29</v>
+      </c>
+      <c r="B98" t="n">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D98" t="n">
+        <v>33</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H98" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I98" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K98" t="n">
+        <v>147</v>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>co</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>29</v>
+      </c>
+      <c r="B99" t="n">
+        <v>5</v>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D99" t="n">
+        <v>33</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H99" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I99" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K99" t="n">
+        <v>148</v>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>no2</t>
+        </is>
+      </c>
+      <c r="M99" t="n">
+        <v>26.1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29</v>
+      </c>
+      <c r="B100" t="n">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>45759.54166666666</v>
+      </c>
+      <c r="D100" t="n">
+        <v>33</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>o3</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>waqi</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="H100" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K100" t="n">
+        <v>149</v>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>so2</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>